<commit_message>
document input table read in (using standardized formats)
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/DEMO-INPUT-TABLES/Parent.xlsx
+++ b/DOCUMENTATION/DEMO-INPUT-TABLES/Parent.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/DP4-R/DOCUMENTATION/DEMO-INPUT-TABLES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D3B07C-8628-EE46-8342-51D489D44A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D60D7BB-13C5-624F-928D-F0A21BF9DB55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{C9FF4BE8-38E8-4C4A-AC74-EE9A69DC62CF}"/>
+    <workbookView xWindow="17660" yWindow="1320" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{C9FF4BE8-38E8-4C4A-AC74-EE9A69DC62CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="5-0 to 5-5" sheetId="1" r:id="rId1"/>
-    <sheet name="5-6 to 5-11" sheetId="2" r:id="rId2"/>
+    <sheet name="060" sheetId="1" r:id="rId1"/>
+    <sheet name="066" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" iterate="1" iterateCount="500" calcOnSave="0"/>
   <extLst>
@@ -478,7 +478,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>